<commit_message>
Updating documentation for manual testing
</commit_message>
<xml_diff>
--- a/manual-testing/test-case-template.xlsx
+++ b/manual-testing/test-case-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivana\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivana\Desktop\IvanaStamenkovic_QMAA_Vega_Test\manual-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76C309A-5281-44B1-B3C8-5BB4BCA01C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81E9E61-66B0-486F-9155-84961637F58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,9 +127,6 @@
     <t>the importance of the test case</t>
   </si>
   <si>
-    <t>step-by-step instructions for executing test case</t>
-  </si>
-  <si>
     <t>any specific input data or credentials required for testing</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
   </si>
   <si>
     <t>the ID of the bug report associated with the test case</t>
+  </si>
+  <si>
+    <t>step-by-step instructions for executing the test case</t>
   </si>
 </sst>
 </file>
@@ -612,8 +612,8 @@
   </sheetPr>
   <dimension ref="A1:AB1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19:L20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -898,19 +898,19 @@
         <v>32</v>
       </c>
       <c r="E13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="G13" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="H13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="I13" s="15" t="s">
         <v>38</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>39</v>
       </c>
       <c r="J13" s="17" t="s">
         <v>31</v>
@@ -919,10 +919,10 @@
         <v>30</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M13" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
@@ -4910,7 +4910,7 @@
       <c r="I1008" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H15:H1048576 I14">
+  <conditionalFormatting sqref="I14 H15:H1048576">
     <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Skipped">
       <formula>NOT(ISERROR(SEARCH("Skipped",H14)))</formula>
     </cfRule>

</xml_diff>